<commit_message>
Refactor and add VALUES
</commit_message>
<xml_diff>
--- a/Minimal/Data.xlsx
+++ b/Minimal/Data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\github.com\open-word\DAX\Minimal\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D28C56E9-2262-4A02-BD6E-1D0A02736590}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E8332858-2CAE-4ED7-AB9D-94936D7739B9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-27960" yWindow="8850" windowWidth="21300" windowHeight="9015" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28920" yWindow="1680" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Orders" sheetId="1" r:id="rId1"/>
@@ -36,10 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="28">
-  <si>
-    <t>Product</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="27">
   <si>
     <t>Quantity</t>
   </si>
@@ -80,9 +77,6 @@
     <t>SO03-3</t>
   </si>
   <si>
-    <t>Customer</t>
-  </si>
-  <si>
     <t>CustomerKey</t>
   </si>
   <si>
@@ -120,6 +114,9 @@
   </si>
   <si>
     <t>Amount</t>
+  </si>
+  <si>
+    <t>ProductKey</t>
   </si>
 </sst>
 </file>
@@ -283,7 +280,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -294,7 +291,6 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
@@ -349,13 +345,6 @@
     </dxf>
     <dxf>
       <border outline="0">
-        <bottom style="thin">
-          <color theme="4" tint="0.39997558519241921"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <border outline="0">
         <right style="thin">
           <color theme="4" tint="0.39997558519241921"/>
         </right>
@@ -390,6 +379,13 @@
           <bgColor theme="4" tint="0.79998168889431442"/>
         </patternFill>
       </fill>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <bottom style="thin">
+          <color theme="4" tint="0.39997558519241921"/>
+        </bottom>
+      </border>
     </dxf>
     <dxf>
       <font>
@@ -535,7 +531,7 @@
     <tableColumn id="7" xr3:uid="{D37CE176-5251-40D7-A73B-0622340A7684}" name="SalesOrderKey" dataDxfId="8"/>
     <tableColumn id="8" xr3:uid="{5AF9D6A9-265D-45CE-992D-63285D1A95ED}" name="SalesOrderItemKey" dataDxfId="7"/>
     <tableColumn id="1" xr3:uid="{6EF87348-5115-4DFF-8D9A-95C06681FAD5}" name="CustomerKey" dataDxfId="6"/>
-    <tableColumn id="2" xr3:uid="{FCA88C6B-0898-459A-92A2-3CE0EB8144E2}" name="Product"/>
+    <tableColumn id="2" xr3:uid="{FCA88C6B-0898-459A-92A2-3CE0EB8144E2}" name="ProductKey"/>
     <tableColumn id="3" xr3:uid="{23337A0D-350A-4CDB-9B1C-902E1C40443A}" name="Quantity"/>
     <tableColumn id="4" xr3:uid="{B5472A36-DE24-4F68-89AF-FF6AF6500AB9}" name="Price"/>
   </tableColumns>
@@ -544,10 +540,10 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{F5C0AB77-04CB-426F-B41E-1B839E18EE0B}" name="Customer" displayName="Customer" ref="E3:E7" totalsRowShown="0" headerRowDxfId="5" dataDxfId="4" headerRowBorderDxfId="2" tableBorderDxfId="3" totalsRowBorderDxfId="1">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{F5C0AB77-04CB-426F-B41E-1B839E18EE0B}" name="Customer" displayName="Customer" ref="E3:E7" totalsRowShown="0" headerRowDxfId="5" dataDxfId="3" headerRowBorderDxfId="4" tableBorderDxfId="2" totalsRowBorderDxfId="1">
   <autoFilter ref="E3:E7" xr:uid="{F5C0AB77-04CB-426F-B41E-1B839E18EE0B}"/>
   <tableColumns count="1">
-    <tableColumn id="1" xr3:uid="{3128F681-7098-4FE0-A0C1-534DB4B67C8D}" name="Customer" dataDxfId="0"/>
+    <tableColumn id="1" xr3:uid="{3128F681-7098-4FE0-A0C1-534DB4B67C8D}" name="CustomerKey" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -557,7 +553,7 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{29942184-BDED-4D14-9187-A49EE3A5457A}" name="Product" displayName="Product" ref="F19:F23" totalsRowShown="0">
   <autoFilter ref="F19:F23" xr:uid="{29942184-BDED-4D14-9187-A49EE3A5457A}"/>
   <tableColumns count="1">
-    <tableColumn id="1" xr3:uid="{8E583CF2-D440-4A83-A6C1-683F7A8D2D66}" name="Product"/>
+    <tableColumn id="1" xr3:uid="{8E583CF2-D440-4A83-A6C1-683F7A8D2D66}" name="ProductKey"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -833,82 +829,82 @@
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="3" max="3" width="16.42578125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="18.42578125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="20.28515625" customWidth="1"/>
-    <col min="6" max="6" width="10" customWidth="1"/>
+    <col min="4" max="4" width="20.7109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="15.140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="13.42578125" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="10.85546875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="3:12" x14ac:dyDescent="0.25">
       <c r="E2" s="9" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
     </row>
     <row r="3" spans="3:12" x14ac:dyDescent="0.25">
       <c r="E3" s="7" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="4" spans="3:12" x14ac:dyDescent="0.25">
       <c r="E4" s="4" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
     </row>
     <row r="5" spans="3:12" x14ac:dyDescent="0.25">
       <c r="E5" s="4" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
     </row>
     <row r="6" spans="3:12" x14ac:dyDescent="0.25">
       <c r="E6" s="8" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
     </row>
     <row r="7" spans="3:12" x14ac:dyDescent="0.25">
-      <c r="E7" s="10" t="s">
-        <v>25</v>
+      <c r="E7" s="8" t="s">
+        <v>23</v>
       </c>
     </row>
     <row r="9" spans="3:12" x14ac:dyDescent="0.25">
       <c r="C9" s="9" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
     </row>
     <row r="10" spans="3:12" x14ac:dyDescent="0.25">
       <c r="C10" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="D10" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="D10" s="1" t="s">
-        <v>7</v>
-      </c>
       <c r="E10" s="2" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="F10" t="s">
+        <v>26</v>
+      </c>
+      <c r="G10" t="s">
         <v>0</v>
       </c>
-      <c r="G10" t="s">
+      <c r="H10" t="s">
         <v>1</v>
       </c>
-      <c r="H10" t="s">
-        <v>2</v>
-      </c>
-      <c r="L10" s="11" t="s">
-        <v>27</v>
+      <c r="L10" s="10" t="s">
+        <v>25</v>
       </c>
     </row>
     <row r="11" spans="3:12" x14ac:dyDescent="0.25">
       <c r="C11" s="3" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D11" s="3" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E11" s="4" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="F11" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="G11">
         <v>1</v>
@@ -916,23 +912,23 @@
       <c r="H11">
         <v>10</v>
       </c>
-      <c r="L11" s="12">
+      <c r="L11" s="11">
         <f>Sales[[#This Row],[Quantity]]*Sales[[#This Row],[Price]]</f>
         <v>10</v>
       </c>
     </row>
     <row r="12" spans="3:12" x14ac:dyDescent="0.25">
       <c r="C12" s="5" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D12" s="5" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E12" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="F12" t="s">
         <v>17</v>
-      </c>
-      <c r="F12" t="s">
-        <v>19</v>
       </c>
       <c r="G12">
         <v>1</v>
@@ -940,23 +936,23 @@
       <c r="H12">
         <v>10</v>
       </c>
-      <c r="L12" s="13">
+      <c r="L12" s="12">
         <f>Sales[[#This Row],[Quantity]]*Sales[[#This Row],[Price]]</f>
         <v>10</v>
       </c>
     </row>
     <row r="13" spans="3:12" x14ac:dyDescent="0.25">
       <c r="C13" s="5" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D13" s="3" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E13" s="6" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="F13" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="G13">
         <v>2</v>
@@ -964,23 +960,23 @@
       <c r="H13">
         <v>20</v>
       </c>
-      <c r="L13" s="13">
+      <c r="L13" s="12">
         <f>Sales[[#This Row],[Quantity]]*Sales[[#This Row],[Price]]</f>
         <v>40</v>
       </c>
     </row>
     <row r="14" spans="3:12" x14ac:dyDescent="0.25">
       <c r="C14" s="3" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D14" s="5" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="E14" s="6" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="F14" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="G14">
         <v>1</v>
@@ -988,23 +984,23 @@
       <c r="H14">
         <v>10</v>
       </c>
-      <c r="L14" s="13">
+      <c r="L14" s="12">
         <f>Sales[[#This Row],[Quantity]]*Sales[[#This Row],[Price]]</f>
         <v>10</v>
       </c>
     </row>
     <row r="15" spans="3:12" x14ac:dyDescent="0.25">
       <c r="C15" s="3" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D15" s="3" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="E15" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="F15" t="s">
         <v>18</v>
-      </c>
-      <c r="F15" t="s">
-        <v>20</v>
       </c>
       <c r="G15">
         <v>2</v>
@@ -1012,23 +1008,23 @@
       <c r="H15">
         <v>20</v>
       </c>
-      <c r="L15" s="13">
+      <c r="L15" s="12">
         <f>Sales[[#This Row],[Quantity]]*Sales[[#This Row],[Price]]</f>
         <v>40</v>
       </c>
     </row>
     <row r="16" spans="3:12" x14ac:dyDescent="0.25">
       <c r="C16" s="3" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D16" s="5" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="E16" s="6" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="F16" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="G16">
         <v>3</v>
@@ -1036,39 +1032,39 @@
       <c r="H16">
         <v>30</v>
       </c>
-      <c r="L16" s="14">
+      <c r="L16" s="13">
         <f>Sales[[#This Row],[Quantity]]*Sales[[#This Row],[Price]]</f>
         <v>90</v>
       </c>
     </row>
     <row r="18" spans="6:6" x14ac:dyDescent="0.25">
       <c r="F18" s="9" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
     </row>
     <row r="19" spans="6:6" x14ac:dyDescent="0.25">
       <c r="F19" t="s">
-        <v>0</v>
+        <v>26</v>
       </c>
     </row>
     <row r="20" spans="6:6" x14ac:dyDescent="0.25">
       <c r="F20" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
     </row>
     <row r="21" spans="6:6" x14ac:dyDescent="0.25">
       <c r="F21" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
     </row>
     <row r="22" spans="6:6" x14ac:dyDescent="0.25">
       <c r="F22" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
     </row>
     <row r="23" spans="6:6" x14ac:dyDescent="0.25">
       <c r="F23" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Complete PB-427 (Introducing CALCULATE and CALCULATETABLE)
</commit_message>
<xml_diff>
--- a/Minimal/Data.xlsx
+++ b/Minimal/Data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\github.com\open-word\DAX\Minimal\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E8332858-2CAE-4ED7-AB9D-94936D7739B9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CA94522F-180E-4221-A326-430E5BCA833C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="1680" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="33">
   <si>
     <t>Quantity</t>
   </si>
@@ -117,6 +117,24 @@
   </si>
   <si>
     <t>ProductKey</t>
+  </si>
+  <si>
+    <t>Color</t>
+  </si>
+  <si>
+    <t>Red</t>
+  </si>
+  <si>
+    <t>Blue</t>
+  </si>
+  <si>
+    <t>Size</t>
+  </si>
+  <si>
+    <t>L</t>
+  </si>
+  <si>
+    <t>M</t>
   </si>
 </sst>
 </file>
@@ -550,10 +568,12 @@
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{29942184-BDED-4D14-9187-A49EE3A5457A}" name="Product" displayName="Product" ref="F19:F23" totalsRowShown="0">
-  <autoFilter ref="F19:F23" xr:uid="{29942184-BDED-4D14-9187-A49EE3A5457A}"/>
-  <tableColumns count="1">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{29942184-BDED-4D14-9187-A49EE3A5457A}" name="Product" displayName="Product" ref="F19:H23" totalsRowShown="0">
+  <autoFilter ref="F19:H23" xr:uid="{29942184-BDED-4D14-9187-A49EE3A5457A}"/>
+  <tableColumns count="3">
     <tableColumn id="1" xr3:uid="{8E583CF2-D440-4A83-A6C1-683F7A8D2D66}" name="ProductKey"/>
+    <tableColumn id="2" xr3:uid="{EA0897D6-3274-4697-967C-CD6479893811}" name="Color"/>
+    <tableColumn id="3" xr3:uid="{EEB1BD55-F29D-41CC-AA6A-A79C660EA423}" name="Size"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -824,7 +844,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="C2:L23"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0"/>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+      <selection activeCell="H24" sqref="H24"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -1037,34 +1059,64 @@
         <v>90</v>
       </c>
     </row>
-    <row r="18" spans="6:6" x14ac:dyDescent="0.25">
+    <row r="18" spans="6:8" x14ac:dyDescent="0.25">
       <c r="F18" s="9" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="19" spans="6:6" x14ac:dyDescent="0.25">
+    <row r="19" spans="6:8" x14ac:dyDescent="0.25">
       <c r="F19" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="20" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="G19" t="s">
+        <v>27</v>
+      </c>
+      <c r="H19" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="20" spans="6:8" x14ac:dyDescent="0.25">
       <c r="F20" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="21" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="G20" t="s">
+        <v>28</v>
+      </c>
+      <c r="H20" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="21" spans="6:8" x14ac:dyDescent="0.25">
       <c r="F21" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="22" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="G21" t="s">
+        <v>28</v>
+      </c>
+      <c r="H21" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="22" spans="6:8" x14ac:dyDescent="0.25">
       <c r="F22" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="23" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="G22" t="s">
+        <v>29</v>
+      </c>
+      <c r="H22" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="23" spans="6:8" x14ac:dyDescent="0.25">
       <c r="F23" t="s">
         <v>24</v>
+      </c>
+      <c r="G23" t="s">
+        <v>29</v>
+      </c>
+      <c r="H23" t="s">
+        <v>31</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Understanding SUMMARIZECOLUMNS auto-exists behavior
</commit_message>
<xml_diff>
--- a/Minimal/Data.xlsx
+++ b/Minimal/Data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\github.com\open-word\DAX\Minimal\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EADA94F1-E2E1-476C-B197-023D63DFC614}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{37FE93FC-9A95-4720-8814-5AA2266F986F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="14400" windowHeight="18000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1950" yWindow="1950" windowWidth="21600" windowHeight="13185" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Orders" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="45">
   <si>
     <t>Quantity</t>
   </si>
@@ -138,6 +138,39 @@
   </si>
   <si>
     <t>Sales</t>
+  </si>
+  <si>
+    <t>CustomerType</t>
+  </si>
+  <si>
+    <t>A</t>
+  </si>
+  <si>
+    <t>B</t>
+  </si>
+  <si>
+    <t>Subcategory</t>
+  </si>
+  <si>
+    <t>Category</t>
+  </si>
+  <si>
+    <t>Cat 4</t>
+  </si>
+  <si>
+    <t>Subcat 4</t>
+  </si>
+  <si>
+    <t>Cat 1</t>
+  </si>
+  <si>
+    <t>Subcat 1</t>
+  </si>
+  <si>
+    <t>Subcat 2</t>
+  </si>
+  <si>
+    <t>Subcat 3</t>
   </si>
 </sst>
 </file>
@@ -301,7 +334,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -316,11 +349,48 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="9">
+  <dxfs count="10">
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor theme="4" tint="0.79998168889431442"/>
+          <bgColor theme="4" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right/>
+        <top style="thin">
+          <color theme="4" tint="0.39997558519241921"/>
+        </top>
+        <bottom style="thin">
+          <color theme="4" tint="0.39997558519241921"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
     <dxf>
       <font>
         <b val="0"/>
@@ -549,9 +619,9 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{19505051-9F5C-4A8C-9D97-CBF734CED51D}" name="Sales" displayName="Sales" ref="C10:H16" totalsRowShown="0">
   <autoFilter ref="C10:H16" xr:uid="{19505051-9F5C-4A8C-9D97-CBF734CED51D}"/>
   <tableColumns count="6">
-    <tableColumn id="7" xr3:uid="{D37CE176-5251-40D7-A73B-0622340A7684}" name="SalesOrderKey" dataDxfId="8"/>
-    <tableColumn id="8" xr3:uid="{5AF9D6A9-265D-45CE-992D-63285D1A95ED}" name="SalesOrderItemKey" dataDxfId="7"/>
-    <tableColumn id="1" xr3:uid="{6EF87348-5115-4DFF-8D9A-95C06681FAD5}" name="CustomerKey" dataDxfId="6"/>
+    <tableColumn id="7" xr3:uid="{D37CE176-5251-40D7-A73B-0622340A7684}" name="SalesOrderKey" dataDxfId="9"/>
+    <tableColumn id="8" xr3:uid="{5AF9D6A9-265D-45CE-992D-63285D1A95ED}" name="SalesOrderItemKey" dataDxfId="8"/>
+    <tableColumn id="1" xr3:uid="{6EF87348-5115-4DFF-8D9A-95C06681FAD5}" name="CustomerKey" dataDxfId="7"/>
     <tableColumn id="2" xr3:uid="{FCA88C6B-0898-459A-92A2-3CE0EB8144E2}" name="ProductKey"/>
     <tableColumn id="3" xr3:uid="{23337A0D-350A-4CDB-9B1C-902E1C40443A}" name="Quantity"/>
     <tableColumn id="4" xr3:uid="{B5472A36-DE24-4F68-89AF-FF6AF6500AB9}" name="Net Price"/>
@@ -561,23 +631,26 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{F5C0AB77-04CB-426F-B41E-1B839E18EE0B}" name="Customer" displayName="Customer" ref="E3:E7" totalsRowShown="0" headerRowDxfId="5" dataDxfId="3" headerRowBorderDxfId="4" tableBorderDxfId="2" totalsRowBorderDxfId="1">
-  <autoFilter ref="E3:E7" xr:uid="{F5C0AB77-04CB-426F-B41E-1B839E18EE0B}"/>
-  <tableColumns count="1">
-    <tableColumn id="1" xr3:uid="{3128F681-7098-4FE0-A0C1-534DB4B67C8D}" name="CustomerKey" dataDxfId="0"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{F5C0AB77-04CB-426F-B41E-1B839E18EE0B}" name="Customer" displayName="Customer" ref="E3:F7" totalsRowShown="0" headerRowDxfId="6" dataDxfId="4" headerRowBorderDxfId="5" tableBorderDxfId="3" totalsRowBorderDxfId="2">
+  <autoFilter ref="E3:F7" xr:uid="{F5C0AB77-04CB-426F-B41E-1B839E18EE0B}"/>
+  <tableColumns count="2">
+    <tableColumn id="1" xr3:uid="{3128F681-7098-4FE0-A0C1-534DB4B67C8D}" name="CustomerKey" dataDxfId="1"/>
+    <tableColumn id="2" xr3:uid="{9F2E657A-AA3E-47AE-9EB9-E28D93554AB0}" name="CustomerType" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{29942184-BDED-4D14-9187-A49EE3A5457A}" name="Product" displayName="Product" ref="F19:I23" totalsRowShown="0">
-  <autoFilter ref="F19:I23" xr:uid="{29942184-BDED-4D14-9187-A49EE3A5457A}"/>
-  <tableColumns count="4">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{29942184-BDED-4D14-9187-A49EE3A5457A}" name="Product" displayName="Product" ref="F19:K23" totalsRowShown="0">
+  <autoFilter ref="F19:K23" xr:uid="{29942184-BDED-4D14-9187-A49EE3A5457A}"/>
+  <tableColumns count="6">
     <tableColumn id="1" xr3:uid="{8E583CF2-D440-4A83-A6C1-683F7A8D2D66}" name="ProductKey"/>
     <tableColumn id="2" xr3:uid="{1F8522C5-3BD8-493B-B610-D105A6D84097}" name="Color"/>
     <tableColumn id="3" xr3:uid="{9B69AA69-8ECB-42CC-9453-F0842BEE8F53}" name="Size"/>
     <tableColumn id="4" xr3:uid="{60E9A36E-03F1-4A4C-9637-DA3D5D610867}" name="Price"/>
+    <tableColumn id="5" xr3:uid="{9DACC361-C3E6-4FDE-86D5-14121A1A4F93}" name="Category"/>
+    <tableColumn id="6" xr3:uid="{9E775E1E-711B-4933-818F-8032C4E18C54}" name="Subcategory"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -848,7 +921,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="C2:L23"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0"/>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+      <selection activeCell="L22" sqref="L22"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -858,6 +933,8 @@
     <col min="6" max="6" width="13.42578125" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="10.85546875" customWidth="1"/>
     <col min="8" max="9" width="11.42578125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="11.140625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="14.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="3:12" x14ac:dyDescent="0.25">
@@ -869,26 +946,41 @@
       <c r="E3" s="7" t="s">
         <v>13</v>
       </c>
+      <c r="F3" s="7" t="s">
+        <v>34</v>
+      </c>
     </row>
     <row r="4" spans="3:12" x14ac:dyDescent="0.25">
       <c r="E4" s="4" t="s">
         <v>14</v>
       </c>
+      <c r="F4" s="14" t="s">
+        <v>35</v>
+      </c>
     </row>
     <row r="5" spans="3:12" x14ac:dyDescent="0.25">
       <c r="E5" s="4" t="s">
         <v>15</v>
       </c>
+      <c r="F5" s="4" t="s">
+        <v>35</v>
+      </c>
     </row>
     <row r="6" spans="3:12" x14ac:dyDescent="0.25">
       <c r="E6" s="8" t="s">
         <v>16</v>
       </c>
+      <c r="F6" s="4" t="s">
+        <v>35</v>
+      </c>
     </row>
     <row r="7" spans="3:12" x14ac:dyDescent="0.25">
       <c r="E7" s="8" t="s">
         <v>20</v>
       </c>
+      <c r="F7" s="8" t="s">
+        <v>36</v>
+      </c>
     </row>
     <row r="9" spans="3:12" x14ac:dyDescent="0.25">
       <c r="C9" s="9" t="s">
@@ -1062,12 +1154,12 @@
         <v>81</v>
       </c>
     </row>
-    <row r="18" spans="6:9" x14ac:dyDescent="0.25">
+    <row r="18" spans="6:11" x14ac:dyDescent="0.25">
       <c r="F18" s="9" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="19" spans="6:9" x14ac:dyDescent="0.25">
+    <row r="19" spans="6:11" x14ac:dyDescent="0.25">
       <c r="F19" t="s">
         <v>23</v>
       </c>
@@ -1080,8 +1172,14 @@
       <c r="I19" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="20" spans="6:9" x14ac:dyDescent="0.25">
+      <c r="J19" t="s">
+        <v>38</v>
+      </c>
+      <c r="K19" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="20" spans="6:11" x14ac:dyDescent="0.25">
       <c r="F20" t="s">
         <v>17</v>
       </c>
@@ -1094,8 +1192,14 @@
       <c r="I20">
         <v>10</v>
       </c>
-    </row>
-    <row r="21" spans="6:9" x14ac:dyDescent="0.25">
+      <c r="J20" t="s">
+        <v>41</v>
+      </c>
+      <c r="K20" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="21" spans="6:11" x14ac:dyDescent="0.25">
       <c r="F21" t="s">
         <v>18</v>
       </c>
@@ -1108,8 +1212,14 @@
       <c r="I21">
         <v>20</v>
       </c>
-    </row>
-    <row r="22" spans="6:9" x14ac:dyDescent="0.25">
+      <c r="J21" t="s">
+        <v>41</v>
+      </c>
+      <c r="K21" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="22" spans="6:11" x14ac:dyDescent="0.25">
       <c r="F22" t="s">
         <v>19</v>
       </c>
@@ -1122,8 +1232,14 @@
       <c r="I22">
         <v>30</v>
       </c>
-    </row>
-    <row r="23" spans="6:9" x14ac:dyDescent="0.25">
+      <c r="J22" t="s">
+        <v>41</v>
+      </c>
+      <c r="K22" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="23" spans="6:11" x14ac:dyDescent="0.25">
       <c r="F23" t="s">
         <v>21</v>
       </c>
@@ -1134,6 +1250,12 @@
         <v>29</v>
       </c>
       <c r="I23">
+        <v>40</v>
+      </c>
+      <c r="J23" t="s">
+        <v>39</v>
+      </c>
+      <c r="K23" t="s">
         <v>40</v>
       </c>
     </row>

</xml_diff>